<commit_message>
add reported comorbidities figures
</commit_message>
<xml_diff>
--- a/data/metadata/table_of_contents.xlsx
+++ b/data/metadata/table_of_contents.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u0148249\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u0133728\Desktop\NEED-GQ\data\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B72A0BC-EDAA-4AE1-84DF-D2CB6D1B1968}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BA0D76B-F356-4F7F-B193-50638DC8526C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="figures" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="75">
   <si>
     <t>id</t>
   </si>
@@ -258,13 +258,10 @@
     <t>Recruitment poster used in the study</t>
   </si>
   <si>
-    <t xml:space="preserve">Shouldn't be made in R, can be manually </t>
-  </si>
-  <si>
-    <t>Column1</t>
-  </si>
-  <si>
     <t>impact_work</t>
+  </si>
+  <si>
+    <t>r-generated</t>
   </si>
 </sst>
 </file>
@@ -404,7 +401,7 @@
     <tableColumn id="2" xr3:uid="{1EE57105-AB53-462A-BB90-78D01B003ED3}" name="name"/>
     <tableColumn id="3" xr3:uid="{61BFBAD0-6DFE-4DC8-ADB8-F03F6347E6EB}" name="caption"/>
     <tableColumn id="4" xr3:uid="{0CA7BEB5-C2D5-4705-A460-B8E01FE605F7}" name="Not from Survey"/>
-    <tableColumn id="5" xr3:uid="{40BF8502-D70B-43C6-BE15-BAF9F33C122A}" name="Column1"/>
+    <tableColumn id="5" xr3:uid="{40BF8502-D70B-43C6-BE15-BAF9F33C122A}" name="r-generated"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -712,18 +709,18 @@
   <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="32.5546875" customWidth="1"/>
+    <col min="2" max="2" width="32.5703125" customWidth="1"/>
     <col min="3" max="3" width="130" customWidth="1"/>
-    <col min="4" max="4" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="34.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -740,7 +737,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -753,8 +750,11 @@
       <c r="D2" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -767,8 +767,11 @@
       <c r="D3" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -781,8 +784,11 @@
       <c r="D4" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -795,8 +801,11 @@
       <c r="D5" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -809,8 +818,11 @@
       <c r="D6" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -820,11 +832,11 @@
       <c r="C7" t="s">
         <v>12</v>
       </c>
-      <c r="E7" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -834,8 +846,11 @@
       <c r="C8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -845,8 +860,11 @@
       <c r="C9" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -856,8 +874,11 @@
       <c r="C10" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -867,8 +888,11 @@
       <c r="C11" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -878,8 +902,11 @@
       <c r="C12" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -889,8 +916,11 @@
       <c r="C13" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -900,8 +930,11 @@
       <c r="C14" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -911,8 +944,11 @@
       <c r="C15" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -922,8 +958,11 @@
       <c r="C16" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -933,8 +972,11 @@
       <c r="C17" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -944,8 +986,11 @@
       <c r="C18" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -955,8 +1000,11 @@
       <c r="C19" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -966,8 +1014,11 @@
       <c r="C20" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -977,8 +1028,11 @@
       <c r="C21" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -988,8 +1042,11 @@
       <c r="C22" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -999,8 +1056,11 @@
       <c r="C23" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1010,8 +1070,11 @@
       <c r="C24" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1021,8 +1084,11 @@
       <c r="C25" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1032,8 +1098,11 @@
       <c r="C26" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1043,16 +1112,22 @@
       <c r="C27" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1062,8 +1137,11 @@
       <c r="C29" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1073,11 +1151,15 @@
       <c r="C30" t="s">
         <v>56</v>
       </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1090,13 +1172,13 @@
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="28.6640625" customWidth="1"/>
-    <col min="3" max="3" width="61.44140625" customWidth="1"/>
+    <col min="2" max="2" width="28.7109375" customWidth="1"/>
+    <col min="3" max="3" width="61.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1107,7 +1189,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1118,7 +1200,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1129,7 +1211,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1140,7 +1222,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1151,7 +1233,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1162,7 +1244,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
Add variables to use
</commit_message>
<xml_diff>
--- a/data/metadata/table_of_contents.xlsx
+++ b/data/metadata/table_of_contents.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u0133728\Desktop\NEED-GQ\data\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8A98E03-6163-40B1-924A-B9E2F320BAE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3165F164-6134-49F2-A9A7-C92861137290}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="78">
   <si>
     <t>id</t>
   </si>
@@ -261,7 +261,16 @@
     <t>impact_work</t>
   </si>
   <si>
-    <t>r-generated</t>
+    <t>variables to use</t>
+  </si>
+  <si>
+    <t>DSD1_A1 to DSD1_A12</t>
+  </si>
+  <si>
+    <t>D15_*</t>
+  </si>
+  <si>
+    <t>HC5_SQ*</t>
   </si>
 </sst>
 </file>
@@ -318,7 +327,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -326,11 +335,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="5">
+    <dxf>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -394,26 +415,27 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C882692D-3398-4514-8DDD-E8CA4CDD04D9}" name="Table1" displayName="Table1" ref="A1:E30" totalsRowShown="0" headerRowDxfId="3" headerRowBorderDxfId="2" tableBorderDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C882692D-3398-4514-8DDD-E8CA4CDD04D9}" name="Table1" displayName="Table1" ref="A1:E30" totalsRowShown="0" headerRowDxfId="4" headerRowBorderDxfId="3" tableBorderDxfId="2">
   <autoFilter ref="A1:E30" xr:uid="{C882692D-3398-4514-8DDD-E8CA4CDD04D9}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{2D79A610-9B2F-492C-9F74-F56FC8A551EB}" name="id"/>
     <tableColumn id="2" xr3:uid="{1EE57105-AB53-462A-BB90-78D01B003ED3}" name="name"/>
-    <tableColumn id="3" xr3:uid="{61BFBAD0-6DFE-4DC8-ADB8-F03F6347E6EB}" name="caption"/>
+    <tableColumn id="3" xr3:uid="{61BFBAD0-6DFE-4DC8-ADB8-F03F6347E6EB}" name="caption" dataDxfId="0"/>
     <tableColumn id="4" xr3:uid="{0CA7BEB5-C2D5-4705-A460-B8E01FE605F7}" name="Not from Survey"/>
-    <tableColumn id="5" xr3:uid="{40BF8502-D70B-43C6-BE15-BAF9F33C122A}" name="r-generated"/>
+    <tableColumn id="5" xr3:uid="{40BF8502-D70B-43C6-BE15-BAF9F33C122A}" name="variables to use"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C17A9586-FAC8-4EE4-95F4-440205A6EC7D}" name="Table2" displayName="Table2" ref="A1:C7" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:C7" xr:uid="{C17A9586-FAC8-4EE4-95F4-440205A6EC7D}"/>
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C17A9586-FAC8-4EE4-95F4-440205A6EC7D}" name="Table2" displayName="Table2" ref="A1:D7" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:D7" xr:uid="{C17A9586-FAC8-4EE4-95F4-440205A6EC7D}"/>
+  <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{066C5649-91CF-49AD-8FB6-64AC3F3280B7}" name="id"/>
     <tableColumn id="2" xr3:uid="{50F684B6-3B5B-4F4E-93B9-6E4A4560312D}" name="name"/>
     <tableColumn id="3" xr3:uid="{224BA299-1288-4D89-9CFE-5B0D8AF9FB96}" name="caption"/>
+    <tableColumn id="4" xr3:uid="{A3FA8997-ABD2-4A98-9D8B-13B42DF1F573}" name="variables to use"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -709,13 +731,13 @@
   <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="E1" sqref="E1:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="32.5703125" customWidth="1"/>
-    <col min="3" max="3" width="130" customWidth="1"/>
+    <col min="3" max="3" width="54.140625" style="3" customWidth="1"/>
     <col min="4" max="4" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="34.5703125" bestFit="1" customWidth="1"/>
   </cols>
@@ -727,7 +749,7 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -737,55 +759,46 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D2" t="s">
         <v>70</v>
       </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D3" t="s">
         <v>70</v>
       </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D4" t="s">
         <v>70</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -795,364 +808,295 @@
       <c r="B5" t="s">
         <v>71</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="3" t="s">
         <v>72</v>
       </c>
       <c r="D5" t="s">
         <v>70</v>
       </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D6" t="s">
         <v>70</v>
       </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>13</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>15</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>17</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>19</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
         <v>21</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
         <v>23</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
         <v>25</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
         <v>27</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
         <v>29</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
         <v>31</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
         <v>33</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
         <v>35</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
         <v>37</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="E20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
         <v>39</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
         <v>41</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
         <v>43</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="E23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
         <v>45</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="E24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
         <v>47</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="E25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
         <v>49</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
         <v>51</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="E27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
         <v>73</v>
       </c>
-      <c r="E28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" t="s">
         <v>53</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="E29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" t="s">
         <v>55</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="E30">
-        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1166,19 +1110,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD118F79-AE35-4A4A-A400-9FE50EC7D930}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="28.7109375" customWidth="1"/>
     <col min="3" max="3" width="61.42578125" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1188,8 +1133,11 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1200,7 +1148,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1211,7 +1159,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1222,7 +1170,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1233,7 +1181,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1244,7 +1192,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
Add comments and included/excluded IDs
</commit_message>
<xml_diff>
--- a/data/metadata/table_of_contents.xlsx
+++ b/data/metadata/table_of_contents.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\0055_Projects\FAR\BA25_Claessens_KCETables\NEED-GQ\data\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A6EDA38-5AAB-4EF6-9678-BEB236A45B2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62EE3188-19FC-4F39-9A9A-5D1EF3CFBFD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11295" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="figures" sheetId="1" r:id="rId1"/>
-    <sheet name="tables" sheetId="2" r:id="rId2"/>
+    <sheet name="general" sheetId="3" r:id="rId1"/>
+    <sheet name="figures" sheetId="1" r:id="rId2"/>
+    <sheet name="tables" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="113">
   <si>
     <t>id</t>
   </si>
@@ -340,6 +341,42 @@
   </si>
   <si>
     <t>impact_sexual_reproductive_health</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please check also figure of psychological symptoms - is this really the same variable and does it make sense to use a different way of visualising? </t>
+  </si>
+  <si>
+    <t>HC3, HC4</t>
+  </si>
+  <si>
+    <t>D6</t>
+  </si>
+  <si>
+    <t>NOT SURVEY</t>
+  </si>
+  <si>
+    <t>H6, H12</t>
+  </si>
+  <si>
+    <t>HC3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. isn't it general practice to mention both the absolute and the relative value of responses? In some graphs the y-axis shows the absolute number, but it is not explicitly used in the balk itself. </t>
+  </si>
+  <si>
+    <t>2. In some cases I felt like the title didn't really match the variables presented. E.g. satisfaction with information: always/sometimes/never - but lets wait what KCE finds about these figures to change it</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. I don't see how it is possible that the N for the EQ-5D questions are differing between the different levels </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4. In all figures you say 'number of patients" while I prefer to use the term 'respondent' can you change it in every figure? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5. If there is "i don't know" as a answer option, put this one on the bottem, because its not really one of the real categories </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6. make all 'i don't know' categories grey </t>
   </si>
 </sst>
 </file>
@@ -506,13 +543,14 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C17A9586-FAC8-4EE4-95F4-440205A6EC7D}" name="Table2" displayName="Table2" ref="A1:D7" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:D7" xr:uid="{C17A9586-FAC8-4EE4-95F4-440205A6EC7D}"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C17A9586-FAC8-4EE4-95F4-440205A6EC7D}" name="Table2" displayName="Table2" ref="A1:E7" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:E7" xr:uid="{C17A9586-FAC8-4EE4-95F4-440205A6EC7D}"/>
+  <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{066C5649-91CF-49AD-8FB6-64AC3F3280B7}" name="id"/>
     <tableColumn id="2" xr3:uid="{50F684B6-3B5B-4F4E-93B9-6E4A4560312D}" name="name"/>
     <tableColumn id="3" xr3:uid="{224BA299-1288-4D89-9CFE-5B0D8AF9FB96}" name="caption"/>
     <tableColumn id="4" xr3:uid="{A3FA8997-ABD2-4A98-9D8B-13B42DF1F573}" name="variables to use"/>
+    <tableColumn id="5" xr3:uid="{FFC90A6D-897C-446F-961E-FA84B77780CD}" name="Column1"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -804,11 +842,54 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E12EB676-05A1-429D-9F53-8B551210B6BA}">
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>112</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1255,12 +1336,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD118F79-AE35-4A4A-A400-9FE50EC7D930}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1268,9 +1349,10 @@
     <col min="2" max="2" width="28.7109375" customWidth="1"/>
     <col min="3" max="3" width="61.42578125" customWidth="1"/>
     <col min="4" max="4" width="19.140625" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1283,8 +1365,11 @@
       <c r="D1" s="5" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1294,8 +1379,14 @@
       <c r="C2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1305,8 +1396,11 @@
       <c r="C3" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1316,8 +1410,11 @@
       <c r="C4" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1327,8 +1424,11 @@
       <c r="C5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1338,8 +1438,11 @@
       <c r="C6" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1349,11 +1452,15 @@
       <c r="C7" t="s">
         <v>67</v>
       </c>
+      <c r="D7" t="s">
+        <v>106</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>